<commit_message>
Automatically re-generate list and index
</commit_message>
<xml_diff>
--- a/docs/1a74f8f7b8b7e871b413c4697f68b4401fbacdf0/reviewdates.xlsx
+++ b/docs/1a74f8f7b8b7e871b413c4697f68b4401fbacdf0/reviewdates.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/SARI/Management of Patients with severe acute respiratory infection SARI.pdf</t>
+          <t>Infection_and_sepsis/SARI/Management of patients with SARI-additional Information.pdf</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/SARI/Management of patients with SARI-additional Information.pdf</t>
+          <t>Infection_and_sepsis/SARI/Suspected Influeza A-H7N9 Guideline.pdf</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/SARI/Suspected Influeza A-H7N9 Guideline.pdf</t>
+          <t>Infection_and_sepsis/SARI/Management of Patients with severe acute respiratory infection SARI.pdf</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -772,7 +772,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>End_of_life_care/Reasons to report a death to PF.pdf</t>
+          <t>Breathing(Respiratory)/salbutamol and ipratroprium MDI.pdf</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Breathing(Respiratory)/salbutamol and ipratroprium MDI.pdf</t>
+          <t>End_of_life_care/Reasons to report a death to PF.pdf</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -796,7 +796,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Neurological/SOP -  Femoral site care.pdf</t>
+          <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy suctioning cleaning guideline.pdf</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy suctioning cleaning guideline.pdf</t>
+          <t>Neurological/SOP -  Femoral site care.pdf</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Covid-19/WGH/CoVid intubation checklist WGH.pdf</t>
+          <t>Covid-19/SJH/SJH COVID19 ITU Intubation Action Card.pdf</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Covid-19/SJH/SJH COVID19 ED Intubation Action Card.pdf</t>
+          <t>Covid-19/WGH/CoVid intubation checklist WGH.pdf</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Diabetes_and_Glucose/Hyperosmolar Hyperglycaemic State.pdf</t>
+          <t>Airway/Emergency intubation checklist_em_pub.pdf</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Covid-19/SJH/SJH COVID19 ITU Intubation Action Card.pdf</t>
+          <t>Covid-19/SJH/SJH COVID19 ED Intubation Action Card.pdf</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -928,7 +928,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Airway/Emergency intubation checklist_em_pub.pdf</t>
+          <t>Diabetes_and_Glucose/Hyperosmolar Hyperglycaemic State.pdf</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Delirium/Risk assessment posi mit.pdf</t>
+          <t>Delirium/Managing a Potentially Violent Patient.pdf</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1036,7 +1036,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/SOP Ultrasound Cleaning.pdf</t>
+          <t>Delirium/Risk assessment posi mit.pdf</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Delirium/Managing a Potentially Violent Patient.pdf</t>
+          <t>Infection_and_sepsis/SOP Ultrasound Cleaning.pdf</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1060,7 +1060,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Neurological/Sub arachnoid haemorrhage management.pdf</t>
+          <t>Breathing(Respiratory)/HFNO.pdf</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1072,7 +1072,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Airway/McGrath Mac.pdf</t>
+          <t>Drugs/ketamine_in_asthma.pdf</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>GI_Liver_and_Transplant/Treatment of constipation.pdf</t>
+          <t>Delirium/Drugs Causing Delirium and Agitiation.pdf</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1108,7 +1108,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Delirium/Drugs Causing Delirium and Agitiation.pdf</t>
+          <t>Airway/McGrath Mac.pdf</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1120,7 +1120,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Breathing(Respiratory)/HFNO.pdf</t>
+          <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy safety box contents.pdf</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1132,7 +1132,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>GI_Liver_and_Transplant/Abdominal pressure measurement.pdf</t>
+          <t>Neurological/Sub arachnoid haemorrhage management.pdf</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1144,7 +1144,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Airway/Tracheostomy_Laryngectomy/Tracheostomy safety box contents.pdf</t>
+          <t>GI_Liver_and_Transplant/Treatment of constipation.pdf</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Drugs/ketamine_in_asthma.pdf</t>
+          <t>GI_Liver_and_Transplant/Abdominal pressure measurement.pdf</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1180,7 +1180,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>GI_Liver_and_Transplant/stress ulcer prophylaxis.pdf</t>
+          <t>Drugs/anidulafungin.pdf</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1204,7 +1204,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Drugs/anidulafungin.pdf</t>
+          <t>GI_Liver_and_Transplant/stress ulcer prophylaxis.pdf</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1240,7 +1240,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Breathing(Respiratory)/Equipment/HFNO Set Up.pdf</t>
+          <t>Drugs/insulin.pdf</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Drugs/insulin.pdf</t>
+          <t>Breathing(Respiratory)/Equipment/HFNO Set Up.pdf</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1312,7 +1312,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Neurological/SOP for review of Neurosurgical patients in ITU by neurosurgical team.pdf</t>
+          <t>Post_op_care/Epidural Haematoma.pdf</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Breathing(Respiratory)/Equipment/T piece Y piece.pdf</t>
+          <t>Drugs/morphine.pdf</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1336,7 +1336,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Drugs/morphine.pdf</t>
+          <t>Breathing(Respiratory)/Equipment/T piece Y piece.pdf</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1348,7 +1348,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Post_op_care/Epidural Haematoma.pdf</t>
+          <t>Neurological/SOP for review of Neurosurgical patients in ITU by neurosurgical team.pdf</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1360,7 +1360,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Policies_and_admin/General Critical Care Interaction with HEPMA_pub.pdf</t>
+          <t>Infection_and_sepsis/BAL and MiniBAL standardised procedure.pdf</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1372,7 +1372,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Drugs/atracurium.pdf</t>
+          <t>Policies_and_admin/General Critical Care Interaction with HEPMA_pub.pdf</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1384,7 +1384,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/BAL and MiniBAL standardised procedure.pdf</t>
+          <t>Drugs/atracurium.pdf</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1468,7 +1468,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Drugs/phenylephrine.pdf</t>
+          <t>Post_op_care/Post op care pharyngo-laryngo-oesphagectomy PLOG.pdf</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1480,7 +1480,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Drugs/amiodarone.pdf</t>
+          <t>Drugs/phenylephrine.pdf</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Post_op_care/Post op care pharyngo-laryngo-oesphagectomy PLOG.pdf</t>
+          <t>Drugs/amiodarone.pdf</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>GI_Liver_and_Transplant/Nasogastric feeding protocol.pdf</t>
+          <t>Drugs/potassium.pdf</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1528,7 +1528,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Drugs/potassium.pdf</t>
+          <t>GI_Liver_and_Transplant/Nasogastric feeding protocol.pdf</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/Antibiotic doses in CVVHD.pdf</t>
+          <t>Drugs/Antibiotic doses in CVVHD.pdf</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1576,7 +1576,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Renal_and_Urology/Antibiotic doses in CVVHD.pdf</t>
+          <t>Infection_and_sepsis/Antibiotic doses in CVVHD.pdf</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1600,7 +1600,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Drugs/Antibiotic doses in CVVHD.pdf</t>
+          <t>Renal_and_Urology/Antibiotic doses in CVVHD.pdf</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>GI_Liver_and_Transplant/Nasojejunal feeding protocol.pdf</t>
+          <t>ECLS/RIE ECLS Anti Xa Protocol.pdf</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>ECLS/RIE ECLS Anti Xa Protocol.pdf</t>
+          <t>Drugs/calcium.pdf</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1648,7 +1648,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>GI_Liver_and_Transplant/Jejunostomy feeding protocol.pdf</t>
+          <t>GI_Liver_and_Transplant/Nasojejunal feeding protocol.pdf</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1660,7 +1660,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Drugs/calcium.pdf</t>
+          <t>GI_Liver_and_Transplant/Jejunostomy feeding protocol.pdf</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1683,7 +1683,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/Winter Infections Stepdown Guidance.pdf</t>
+          <t>Neurological/Management of traumatic brain injury.pdf</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -1695,7 +1695,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Drugs/vasopressin organ donation.pdf</t>
+          <t>Neurological/Critical Care MRI Procedure_pub.pdf</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1707,7 +1707,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>End_of_life_care/CMO &amp; NRS Guidance for Doctors completing MCCD - Sept 22.pdf</t>
+          <t>Ethics_and_Law/DNACPR policy for Scotland.pdf</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -1719,7 +1719,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Drugs/nicardipine.pdf</t>
+          <t>Drugs/vasopressin_sepsis.pdf</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1731,7 +1731,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Ethics_and_Law/DNACPR policy for Scotland.pdf</t>
+          <t>Organ_donation/Organ Retrieval SOP.pdf</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1743,7 +1743,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Ethics_and_Law/Care at the End of Life (FICM).pdf</t>
+          <t>Infection_and_sepsis/Winter Infections Stepdown Guidance.pdf</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -1755,7 +1755,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Neurological/Management of traumatic brain injury.pdf</t>
+          <t>Drugs/vasopressin organ donation.pdf</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1767,7 +1767,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Organ_donation/Organ Retrieval SOP.pdf</t>
+          <t>Covid-19/COVID 19 ICM guidance basic goals_June_2022.pdf</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1779,7 +1779,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Neurological/Critical Care MRI Procedure_pub.pdf</t>
+          <t>Ethics_and_Law/Care at the End of Life (FICM).pdf</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1791,7 +1791,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Drugs/vasopressin_sepsis.pdf</t>
+          <t>End_of_life_care/CMO &amp; NRS Guidance for Doctors completing MCCD - Sept 22.pdf</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -1803,7 +1803,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Covid-19/COVID 19 ICM guidance basic goals_June_2022.pdf</t>
+          <t>Drugs/nicardipine.pdf</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -1851,7 +1851,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Covid-19/videos/Donning and Doffing Video.pdf</t>
+          <t>Drugs/ketamine for status epilepticus.pdf</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -1863,7 +1863,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Drugs/thiopentone.pdf</t>
+          <t>Covid-19/videos/Donning and Doffing Video.pdf</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -1887,7 +1887,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Drugs/ketamine for status epilepticus.pdf</t>
+          <t>Drugs/thiopentone.pdf</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -1899,7 +1899,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Breathing(Respiratory)/Equipment/Ventilators Circuits Filters and Closed Suction - Set up and Maintenance.pdf</t>
+          <t>Infection_and_sepsis/Infection indications for IVIG.pdf</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -1911,7 +1911,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/Infection indications for IVIG.pdf</t>
+          <t>Drugs/piperacillin_tazobactam extended_infusion.pdf</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -1923,7 +1923,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Breathing(Respiratory)/Equipment/Bipap V60.pdf</t>
+          <t>Breathing(Respiratory)/CPAP.pdf</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -1935,7 +1935,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Breathing(Respiratory)/CPAP.pdf</t>
+          <t>Breathing(Respiratory)/Equipment/Ventilators Circuits Filters and Closed Suction - Set up and Maintenance.pdf</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -1947,7 +1947,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Drugs/piperacillin_tazobactam extended_infusion.pdf</t>
+          <t>Breathing(Respiratory)/Equipment/Bipap V60.pdf</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -1971,7 +1971,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Transfer/Transfer Outdoors to Garden Guideline.pdf</t>
+          <t>Covid-19/Covid 19 Death Certification Guideline.pdf</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -1983,7 +1983,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Covid-19/Covid 19 Death Certification Guideline.pdf</t>
+          <t>Transfer/Transfer Outdoors to Garden Guideline.pdf</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -2007,7 +2007,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Neurological/Treatment of status epilepticus.pdf</t>
+          <t>Routine_Care/Video Communication.pdf</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2019,7 +2019,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Routine_Care/Video Communication.pdf</t>
+          <t>Neurological/Treatment of status epilepticus.pdf</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -2043,7 +2043,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Drugs/isoprenaline.pdf</t>
+          <t>Cardiovascular/Cardiogenic Shock.pdf</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2055,7 +2055,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Cardiovascular/Cardiogenic Shock.pdf</t>
+          <t>Drugs/isoprenaline.pdf</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2115,7 +2115,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Drugs/aminophylline.pdf</t>
+          <t>Cardiovascular/Management of hypertension within Critical Care.pdf</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2127,7 +2127,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Cardiovascular/Management of hypertension within Critical Care.pdf</t>
+          <t>Drugs/aminophylline.pdf</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2139,7 +2139,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Drugs/pancuronium.pdf</t>
+          <t>Haematology_CAR-T/CRS.pdf</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2163,7 +2163,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Haematology_CAR-T/CRS.pdf</t>
+          <t>Drugs/phenytoin.pdf</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -2187,7 +2187,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Drugs/phenytoin.pdf</t>
+          <t>Drugs/pancuronium.pdf</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2199,7 +2199,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Policies_and_admin/General Critical Care SOP_pub.pdf</t>
+          <t>Drugs/Milrinone.pdf</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -2211,7 +2211,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Drugs/Milrinone.pdf</t>
+          <t>Policies_and_admin/General Critical Care SOP_pub.pdf</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -2247,7 +2247,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Breathing(Respiratory)/Equipment/Passy Muir Valve.pdf</t>
+          <t>Drugs/glyceryl_trinitrate.pdf</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -2283,7 +2283,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Drugs/dexmedetomidine.pdf</t>
+          <t>Breathing(Respiratory)/Equipment/Passy Muir Valve.pdf</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -2295,7 +2295,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Drugs/glyceryl_trinitrate.pdf</t>
+          <t>Drugs/dexmedetomidine.pdf</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -2355,7 +2355,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Drugs/neostigmine.pdf</t>
+          <t>Drugs/vancomycin.pdf</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -2367,7 +2367,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Drugs/vancomycin.pdf</t>
+          <t>Drugs/neostigmine.pdf</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -2379,7 +2379,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Drugs/alteplase for massive PE.pdf</t>
+          <t>Drugs/labetalol.pdf</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -2391,7 +2391,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Drugs/labetalol.pdf</t>
+          <t>Infection_and_sepsis/Initial investigation and management in unidentified Infections.pdf</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -2403,7 +2403,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Infection_and_sepsis/Initial investigation and management in unidentified Infections.pdf</t>
+          <t>Drugs/alteplase for massive PE.pdf</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -2439,7 +2439,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Procedures/Arterial Line insertion for ACCPs.pdf</t>
+          <t>Routine_Care/ICU Eye Care Guideline.pdf</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -2463,7 +2463,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Routine_Care/ICU Eye Care Guideline.pdf</t>
+          <t>Procedures/Arterial Line insertion for ACCPs.pdf</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -2499,7 +2499,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Cardiovascular/Cardiac Output Monitoring _pub.pdf</t>
+          <t>Cardiovascular/Pulmonary_Embolism_and_DVT/Catheter directed thrombolysis of iliofemoral DVT alteplase_pub.pdf</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -2511,7 +2511,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Cardiovascular/Pulmonary_Embolism_and_DVT/Catheter directed thrombolysis of iliofemoral DVT alteplase_pub.pdf</t>
+          <t>Cardiovascular/Cardiac Output Monitoring _pub.pdf</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -2583,7 +2583,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Post_op_care/Prevention and treatment of paraplegia after major aortic procedures.pdf</t>
+          <t>Procedures/ACCPs acquiring initial CVC competencies.pdf</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -2595,7 +2595,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Procedures/ACCPs acquiring initial CVC competencies.pdf</t>
+          <t>Post_op_care/Prevention and treatment of paraplegia after major aortic procedures.pdf</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">

</xml_diff>